<commit_message>
Test Esperienziale e Simulativi
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/RETAIL/test_Ind_Simulativi_RETAIL.xlsx
+++ b/earlywarning-pom/Document/test/RETAIL/test_Ind_Simulativi_RETAIL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="364">
   <si>
     <t>SNDG</t>
   </si>
@@ -1093,6 +1093,24 @@
   </si>
   <si>
     <t>XRA004_2</t>
+  </si>
+  <si>
+    <t>0000000000000492</t>
+  </si>
+  <si>
+    <t>0000000000000493</t>
+  </si>
+  <si>
+    <t>0000000000000494</t>
+  </si>
+  <si>
+    <t>0000000000000495</t>
+  </si>
+  <si>
+    <t>0000000000000496</t>
+  </si>
+  <si>
+    <t>0000000000000497</t>
   </si>
 </sst>
 </file>
@@ -1623,20 +1641,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:CN245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="BF226" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:E1048576"/>
+      <selection pane="bottomRight" activeCell="B245" sqref="B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="27.44140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="33.88671875" style="3" customWidth="1"/>
     <col min="8" max="8" width="24.88671875" style="3" customWidth="1"/>
@@ -1662,16 +1679,15 @@
     <col min="41" max="42" width="28.21875" style="3" customWidth="1"/>
     <col min="43" max="43" width="27.88671875" style="3" customWidth="1"/>
     <col min="44" max="44" width="28.21875" style="3" customWidth="1"/>
-    <col min="45" max="50" width="25.109375" style="3" customWidth="1"/>
-    <col min="51" max="62" width="25.109375" style="3" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="21.21875" style="3" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="21" style="3" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="21.21875" style="3" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="19" style="3" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="18.77734375" style="3" hidden="1" customWidth="1"/>
-    <col min="68" max="69" width="19" style="3" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="17.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="19" style="3" hidden="1" customWidth="1"/>
+    <col min="45" max="62" width="25.109375" style="3" customWidth="1"/>
+    <col min="63" max="63" width="21.21875" style="3" customWidth="1"/>
+    <col min="64" max="64" width="21" style="3" customWidth="1"/>
+    <col min="65" max="65" width="21.21875" style="3" customWidth="1"/>
+    <col min="66" max="66" width="19" style="3" customWidth="1"/>
+    <col min="67" max="67" width="18.77734375" style="3" customWidth="1"/>
+    <col min="68" max="69" width="19" style="3" customWidth="1"/>
+    <col min="70" max="70" width="17.88671875" style="3" customWidth="1"/>
+    <col min="71" max="71" width="19" style="3" customWidth="1"/>
     <col min="72" max="72" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="16.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="74" max="77" width="16.109375" style="3" customWidth="1"/>
@@ -30482,6 +30498,9 @@
       <c r="CN239" s="1"/>
     </row>
     <row r="240" spans="2:92" x14ac:dyDescent="0.3">
+      <c r="B240" s="6" t="s">
+        <v>358</v>
+      </c>
       <c r="C240" s="1">
         <v>230</v>
       </c>
@@ -30591,7 +30610,10 @@
       <c r="CM240" s="1"/>
       <c r="CN240" s="1"/>
     </row>
-    <row r="241" spans="3:92" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:92" x14ac:dyDescent="0.3">
+      <c r="B241" s="6" t="s">
+        <v>359</v>
+      </c>
       <c r="C241" s="1">
         <v>231</v>
       </c>
@@ -30700,7 +30722,10 @@
       <c r="CM241" s="1"/>
       <c r="CN241" s="1"/>
     </row>
-    <row r="242" spans="3:92" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:92" x14ac:dyDescent="0.3">
+      <c r="B242" s="6" t="s">
+        <v>360</v>
+      </c>
       <c r="C242" s="1">
         <v>231</v>
       </c>
@@ -30809,7 +30834,10 @@
       <c r="CM242" s="1"/>
       <c r="CN242" s="1"/>
     </row>
-    <row r="243" spans="3:92" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:92" x14ac:dyDescent="0.3">
+      <c r="B243" s="6" t="s">
+        <v>361</v>
+      </c>
       <c r="C243" s="1">
         <v>231</v>
       </c>
@@ -30919,7 +30947,10 @@
       <c r="CM243" s="1"/>
       <c r="CN243" s="1"/>
     </row>
-    <row r="244" spans="3:92" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:92" x14ac:dyDescent="0.3">
+      <c r="B244" s="6" t="s">
+        <v>362</v>
+      </c>
       <c r="C244" s="1">
         <v>231</v>
       </c>
@@ -31028,7 +31059,10 @@
       <c r="CM244" s="1"/>
       <c r="CN244" s="1"/>
     </row>
-    <row r="245" spans="3:92" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:92" x14ac:dyDescent="0.3">
+      <c r="B245" s="6" t="s">
+        <v>363</v>
+      </c>
       <c r="C245" s="1">
         <v>231</v>
       </c>

</xml_diff>